<commit_message>
volume attempts regression first test
</commit_message>
<xml_diff>
--- a/backend/jupyter/volume_sections/gca_Standardized_coefficients.xlsx
+++ b/backend/jupyter/volume_sections/gca_Standardized_coefficients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\okany\Documents\GitHub\football-simulation-game\backend\jupyter\volume_sections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908477E5-84CF-4839-83B9-5E6206BE0A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9234D68-15F1-454F-8465-F0B13DE80983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2145" windowWidth="23445" windowHeight="12960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4905" yWindow="2970" windowWidth="23445" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="x" sheetId="1" r:id="rId1"/>
@@ -713,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
@@ -4669,7 +4669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>